<commit_message>
Fixes and additions for island comparison cleanup
</commit_message>
<xml_diff>
--- a/Josie/Data/PlantMasterList.xlsx
+++ b/Josie/Data/PlantMasterList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlesage\Dropbox\SBBG\TNC - Gap Analysis\R - Gap Analysis\Josie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlesage\Dropbox\SBBG\TNC - Gap Analysis\R - Gap Analysis\Josie\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED00EDC-C34D-48D4-99E5-58BA300EE0C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4339115-9BB0-4CBF-BA4B-7A2862B222FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15341" uniqueCount="2154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15373" uniqueCount="2158">
   <si>
     <t>assign_by_island</t>
   </si>
@@ -6485,6 +6485,18 @@
   </si>
   <si>
     <t>syn_replace</t>
+  </si>
+  <si>
+    <t>Oenothera guadalupensis subsp. clementina</t>
+  </si>
+  <si>
+    <t>Camissonia guadalupensis subsp. clementina</t>
+  </si>
+  <si>
+    <t>Camissoniopsis guadalupensis</t>
+  </si>
+  <si>
+    <t>Camissoniopsis guadalupensis subsp. clementina</t>
   </si>
 </sst>
 </file>
@@ -6648,7 +6660,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6852,6 +6864,12 @@
         <bgColor rgb="FFD8E4BC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -7028,7 +7046,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -7053,6 +7071,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -7408,11 +7427,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U1921"/>
+  <dimension ref="A1:U1925"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A474" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K495" sqref="K495"/>
+      <pane ySplit="1" topLeftCell="A1913" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1923" sqref="I1923"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -85684,6 +85703,150 @@
         <v>1</v>
       </c>
     </row>
+    <row r="1922" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1922" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1922" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1922" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1922" s="16" t="s">
+        <v>1186</v>
+      </c>
+      <c r="E1922" s="16" t="s">
+        <v>1264</v>
+      </c>
+      <c r="F1922" s="16" t="s">
+        <v>2154</v>
+      </c>
+      <c r="G1922" s="16" t="s">
+        <v>2157</v>
+      </c>
+      <c r="M1922" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1922" s="16"/>
+      <c r="O1922" s="16"/>
+      <c r="P1922" s="16"/>
+      <c r="Q1922" s="16"/>
+      <c r="R1922" s="16"/>
+      <c r="S1922" s="16"/>
+      <c r="T1922" s="16">
+        <v>1</v>
+      </c>
+      <c r="U1922" s="16"/>
+    </row>
+    <row r="1923" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1923" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1923" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1923" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1923" s="16" t="s">
+        <v>1186</v>
+      </c>
+      <c r="E1923" s="16" t="s">
+        <v>1264</v>
+      </c>
+      <c r="F1923" s="16" t="s">
+        <v>2155</v>
+      </c>
+      <c r="G1923" s="16" t="s">
+        <v>2157</v>
+      </c>
+      <c r="M1923" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1923" s="16"/>
+      <c r="O1923" s="16"/>
+      <c r="P1923" s="16"/>
+      <c r="Q1923" s="16"/>
+      <c r="R1923" s="16"/>
+      <c r="S1923" s="16"/>
+      <c r="T1923" s="16">
+        <v>1</v>
+      </c>
+      <c r="U1923" s="16"/>
+    </row>
+    <row r="1924" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1924" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1924" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1924" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1924" s="16" t="s">
+        <v>1186</v>
+      </c>
+      <c r="E1924" s="16" t="s">
+        <v>1264</v>
+      </c>
+      <c r="F1924" s="16" t="s">
+        <v>2156</v>
+      </c>
+      <c r="G1924" s="16" t="s">
+        <v>2157</v>
+      </c>
+      <c r="M1924" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1924" s="16"/>
+      <c r="O1924" s="16"/>
+      <c r="P1924" s="16"/>
+      <c r="Q1924" s="16"/>
+      <c r="R1924" s="16"/>
+      <c r="S1924" s="16"/>
+      <c r="T1924" s="16">
+        <v>1</v>
+      </c>
+      <c r="U1924" s="16"/>
+    </row>
+    <row r="1925" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1925" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1925" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1925" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1925" s="16" t="s">
+        <v>1186</v>
+      </c>
+      <c r="E1925" s="16" t="s">
+        <v>1264</v>
+      </c>
+      <c r="F1925" s="16" t="s">
+        <v>2157</v>
+      </c>
+      <c r="G1925" s="16" t="s">
+        <v>2157</v>
+      </c>
+      <c r="M1925" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1925" s="16"/>
+      <c r="O1925" s="16"/>
+      <c r="P1925" s="16"/>
+      <c r="Q1925" s="16"/>
+      <c r="R1925" s="16"/>
+      <c r="S1925" s="16"/>
+      <c r="T1925" s="16">
+        <v>1</v>
+      </c>
+      <c r="U1925" s="16"/>
+    </row>
   </sheetData>
   <autoFilter ref="N1:U1921" xr:uid="{FCF456B4-550F-44DF-ADC0-DBEA66C0DA5C}"/>
   <sortState ref="A2:U1921">

</xml_diff>